<commit_message>
Search: find number of search iterations (recursive solution)
</commit_message>
<xml_diff>
--- a/Data/Compound Constraints/Compunds.xlsx
+++ b/Data/Compound Constraints/Compunds.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hasnaij\Desktop\Compsci380\MLMSA\Data\Compund Constraints\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hasnaij\Desktop\Compsci380\MLMSA\Data\Compound Constraints\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68FD6EC4-C016-4E78-8870-6AE700F3F66C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF484927-F1B4-4AD5-A3CB-B1EF13A52C20}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,12 +35,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
-    <t>Compund Name</t>
-  </si>
-  <si>
-    <t>Compund Formula</t>
-  </si>
-  <si>
     <t>Mass</t>
   </si>
   <si>
@@ -62,9 +56,6 @@
     <t>Pt</t>
   </si>
   <si>
-    <t>Compound ID</t>
-  </si>
-  <si>
     <t>NH3</t>
   </si>
   <si>
@@ -117,6 +108,15 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Formula</t>
+  </si>
+  <si>
+    <t>ID</t>
   </si>
 </sst>
 </file>
@@ -437,7 +437,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -449,16 +449,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="B1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" t="s">
         <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -466,10 +466,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D2">
         <v>19.018000000000001</v>
@@ -481,10 +481,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D3">
         <v>35.975999999999999</v>
@@ -496,10 +496,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D4">
         <v>195.97200000000001</v>
@@ -511,10 +511,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D5">
         <v>18.033999999999999</v>
@@ -526,10 +526,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D6">
         <v>23.997</v>
@@ -541,10 +541,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D7">
         <v>39.970999999999997</v>
@@ -556,10 +556,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C8" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D8">
         <v>18.010000000000002</v>
@@ -571,10 +571,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C9" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D9">
         <v>17.026</v>
@@ -586,10 +586,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D10">
         <v>19.042000000000002</v>
@@ -601,10 +601,10 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C11" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D11">
         <v>88.986999999999995</v>
@@ -616,10 +616,10 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C12" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D12">
         <v>115.123</v>
@@ -631,10 +631,10 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C13" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D13">
         <v>8566.6460000000006</v>

</xml_diff>